<commit_message>
Add and implemented  LogToFile into the flowchart
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -70,6 +70,12 @@
     <t xml:space="preserve">Timeout_large</t>
   </si>
   <si>
+    <t xml:space="preserve">ApplicationName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DS_AstaGiudiziariaFirenze</t>
+  </si>
+  <si>
     <t xml:space="preserve">MaxRetryNumber</t>
   </si>
   <si>
@@ -188,6 +194,12 @@
   </si>
   <si>
     <t xml:space="preserve">Percorso cartella dove verrà salvato il file csv “FileName_DS”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LogFolderPath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\rodri\Documents\Casa-mutuo\DS_AstaGiudiziariaFirenze\Logs</t>
   </si>
   <si>
     <t xml:space="preserve">Asset</t>
@@ -513,7 +525,7 @@
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -641,10 +653,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -689,125 +701,145 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="5"/>
+    <row r="4" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="1" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+      <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="6" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>41</v>
-      </c>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
@@ -820,56 +852,75 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="7" t="b">
+      <c r="B16" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="C18" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="6" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C21" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="1" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>54</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B20" r:id="rId1" display="https://www.ivgfirenze.it/ricerca/immobili?filter%5Bgenre%5D%5B0%5D=IMMOBILI&amp;filter%5Bcategory%5D%5B0%5D=IMMOBILE%20RESIDENZIALE&amp;filter%5Bcategory%5D%5B1%5D=ALTRA%20CATEGORIA&amp;filter%5Bsubcategory%5D%5B0%5D=APPARTAMENTO&amp;filter%5Bsubcategory%5D%5B1%5D=ABITAZIONE%20IN%20VILLE&amp;filter%5Bsubcategory%5D%5B2%5D=ABITAZIONE%20DI%20TIPO%20CIVILE&amp;filter%5Bstatus%5D%5B0%5D=In%20vendita&amp;filter%5Bprice%5D%5B0%5D=%3C&amp;filter%5Bprice%5D%5B1%5D=400000&amp;filter%5Bvisibile_su%5D%5B0%5D=16&amp;filter%5Bposition%5D=&amp;filter%5Bcity%5D%5B0%5D=Firenze&amp;filter%5Bcity%5D%5B1%5D=Pontassieve&amp;filter%5Bcity%5D%5B2%5D=Scandicci&amp;filter%5Bcity%5D%5B3%5D=Sesto%20Fiorentino&amp;filter%5Bcity%5D%5B4%5D=Fiesole&amp;query=&amp;page=1&amp;rpp=20"/>
-    <hyperlink ref="C20" r:id="rId2" display="https://www.ivgfirenze.it/ricerca/immobili"/>
+    <hyperlink ref="B21" r:id="rId1" display="https://www.ivgfirenze.it/ricerca/immobili?filter%5Bgenre%5D%5B0%5D=IMMOBILI&amp;filter%5Bcategory%5D%5B0%5D=IMMOBILE%20RESIDENZIALE&amp;filter%5Bcategory%5D%5B1%5D=ALTRA%20CATEGORIA&amp;filter%5Bsubcategory%5D%5B0%5D=APPARTAMENTO&amp;filter%5Bsubcategory%5D%5B1%5D=ABITAZIONE%20IN%20VILLE&amp;filter%5Bsubcategory%5D%5B2%5D=ABITAZIONE%20DI%20TIPO%20CIVILE&amp;filter%5Bstatus%5D%5B0%5D=In%20vendita&amp;filter%5Bprice%5D%5B0%5D=%3C&amp;filter%5Bprice%5D%5B1%5D=400000&amp;filter%5Bvisibile_su%5D%5B0%5D=16&amp;filter%5Bposition%5D=&amp;filter%5Bcity%5D%5B0%5D=Firenze&amp;filter%5Bcity%5D%5B1%5D=Pontassieve&amp;filter%5Bcity%5D%5B2%5D=Scandicci&amp;filter%5Bcity%5D%5B3%5D=Sesto%20Fiorentino&amp;filter%5Bcity%5D%5B4%5D=Fiesole&amp;query=&amp;page=1&amp;rpp=20"/>
+    <hyperlink ref="C21" r:id="rId2" display="https://www.ivgfirenze.it/ricerca/immobili"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -905,13 +956,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>

</xml_diff>